<commit_message>
added three js content and GLB File + navigation in three js
</commit_message>
<xml_diff>
--- a/data/material/texts.xlsx
+++ b/data/material/texts.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\21_404\PROJECT\404-nature-not-found\data\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93682B6E-09D8-469C-9C30-7C222401A4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBC1F18-7842-488A-86F5-5083A97D25A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="12735" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Intro" sheetId="2" r:id="rId1"/>
+    <sheet name="Pferde" sheetId="1" r:id="rId1"/>
     <sheet name="Begriffe" sheetId="4" r:id="rId2"/>
-    <sheet name="Pferde" sheetId="1" r:id="rId3"/>
-    <sheet name="Rezepte" sheetId="10" r:id="rId4"/>
-    <sheet name="Autos" sheetId="5" r:id="rId5"/>
-    <sheet name="Strahlwirkung" sheetId="7" r:id="rId6"/>
-    <sheet name="Emscher" sheetId="3" r:id="rId7"/>
+    <sheet name="Strahlwirkung" sheetId="7" r:id="rId3"/>
+    <sheet name="Emscher" sheetId="3" r:id="rId4"/>
+    <sheet name="Intro" sheetId="2" r:id="rId5"/>
+    <sheet name="Fiktion" sheetId="9" r:id="rId6"/>
+    <sheet name="Autos" sheetId="5" r:id="rId7"/>
     <sheet name="Beschwerde" sheetId="6" r:id="rId8"/>
-    <sheet name="Fiktion" sheetId="9" r:id="rId9"/>
+    <sheet name="Rezepte" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1127,20 +1127,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="129.28515625" customWidth="1"/>
-    <col min="2" max="2" width="71.7109375" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" customWidth="1"/>
+    <col min="1" max="1" width="135.5703125" customWidth="1"/>
+    <col min="2" max="2" width="82.85546875" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1160,11 +1160,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="1"/>
+        <v>66</v>
+      </c>
       <c r="D2">
         <v>0</v>
       </c>
@@ -1172,13 +1171,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="B3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" t="s">
-        <v>177</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1187,11 +1185,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D4">
         <v>0</v>
       </c>
@@ -1199,11 +1199,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1"/>
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="D5">
         <v>0</v>
       </c>
@@ -1211,11 +1214,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D6">
         <v>0</v>
       </c>
@@ -1223,11 +1228,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D7">
         <v>0</v>
       </c>
@@ -1235,11 +1242,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="D8">
         <v>0</v>
       </c>
@@ -1247,11 +1256,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1"/>
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="D9">
         <v>0</v>
       </c>
@@ -1259,13 +1271,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C10" t="s">
-        <v>121</v>
+        <v>130</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1274,13 +1286,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="B11" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" t="s">
-        <v>122</v>
+        <v>46</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1289,11 +1300,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D12">
         <v>0</v>
       </c>
@@ -1301,11 +1314,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D13">
         <v>0</v>
       </c>
@@ -1313,11 +1328,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="1"/>
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="D14">
         <v>0</v>
       </c>
@@ -1325,11 +1343,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="1"/>
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="D15">
         <v>0</v>
       </c>
@@ -1337,13 +1358,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+    <row r="16" spans="1:5" s="1" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="B16" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" t="s">
-        <v>178</v>
+        <v>45</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1352,15 +1372,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="1" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="1" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
         <v>0</v>
       </c>
     </row>
@@ -1736,20 +1800,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60854A22-808A-4E1A-91AE-9BEA74945AD8}">
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="135.5703125" customWidth="1"/>
-    <col min="2" max="2" width="82.85546875" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" customWidth="1"/>
+    <col min="1" max="1" width="93.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="90" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1769,10 +1833,804 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2" s="1"/>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E81"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="128.5703125" customWidth="1"/>
+    <col min="2" max="2" width="77.28515625" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="75.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="75.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="66.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="66.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="129.28515625" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>66</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B2" s="1"/>
       <c r="D2">
         <v>0</v>
       </c>
@@ -1780,12 +2638,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>67</v>
-      </c>
+    <row r="3" spans="1:5" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>177</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1794,13 +2653,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B4" s="1"/>
       <c r="D4">
         <v>0</v>
       </c>
@@ -1808,14 +2665,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>93</v>
-      </c>
+    <row r="5" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1"/>
       <c r="D5">
         <v>0</v>
       </c>
@@ -1823,13 +2677,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B6" s="1"/>
       <c r="D6">
         <v>0</v>
       </c>
@@ -1837,13 +2689,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B7" s="1"/>
       <c r="D7">
         <v>0</v>
       </c>
@@ -1851,13 +2701,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>47</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
       <c r="D8">
         <v>0</v>
       </c>
@@ -1865,14 +2713,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>95</v>
-      </c>
+    <row r="9" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
       <c r="D9">
         <v>0</v>
       </c>
@@ -1880,13 +2725,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>94</v>
+        <v>123</v>
+      </c>
+      <c r="C10" t="s">
+        <v>121</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1895,12 +2740,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>1</v>
-      </c>
+    <row r="11" spans="1:5" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>123</v>
+      </c>
+      <c r="C11" t="s">
+        <v>122</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1909,13 +2755,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B12" s="1"/>
       <c r="D12">
         <v>0</v>
       </c>
@@ -1923,13 +2767,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B13" s="1"/>
       <c r="D13">
         <v>0</v>
       </c>
@@ -1937,14 +2779,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>98</v>
-      </c>
+    <row r="14" spans="1:5" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="1"/>
       <c r="D14">
         <v>0</v>
       </c>
@@ -1952,14 +2791,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>97</v>
-      </c>
+    <row r="15" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="1"/>
       <c r="D15">
         <v>0</v>
       </c>
@@ -1967,12 +2803,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>4</v>
-      </c>
+    <row r="16" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>178</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1981,59 +2818,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B17" s="1"/>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="1" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
         <v>0</v>
       </c>
     </row>
@@ -2043,21 +2836,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7AB4E8-874D-432E-A74A-D6E3D309D23E}">
-  <dimension ref="A1:E35"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794DF495-540A-4416-A570-C2CA3FBB663F}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="105.140625" customWidth="1"/>
-    <col min="2" max="2" width="73.28515625" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="1" max="1" width="109.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="86.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2077,40 +2870,40 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>203</v>
+    <row r="2" spans="1:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>180</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="98.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" t="s">
-        <v>74</v>
+    <row r="3" spans="1:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="215.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>73</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -2119,9 +2912,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="210" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>75</v>
+    <row r="5" spans="1:5" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" t="s">
+        <v>181</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -2130,43 +2926,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C6" t="s">
-        <v>77</v>
+    <row r="6" spans="1:5" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" t="s">
-        <v>131</v>
+    <row r="7" spans="1:5" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>183</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="199.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>82</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" t="s">
+        <v>184</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -2175,51 +2968,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="231.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" t="s">
-        <v>79</v>
+        <v>196</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" t="s">
+        <v>185</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" t="s">
-        <v>131</v>
+    <row r="11" spans="1:5" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>186</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>88</v>
+        <v>197</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2228,15 +3024,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="225" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" t="s">
-        <v>131</v>
+    <row r="13" spans="1:5" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>187</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -2245,86 +3038,98 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
+        <v>198</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-    </row>
+    <row r="15" spans="1:5" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" t="s">
+        <v>189</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" t="s">
+        <v>192</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="265.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" t="s">
+        <v>190</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:5" ht="44.45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C96751-A673-424F-84AF-C20C0941739C}">
   <dimension ref="A1:E60"/>
   <sheetViews>
@@ -2772,799 +3577,6 @@
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60854A22-808A-4E1A-91AE-9BEA74945AD8}">
-  <dimension ref="A1:E28"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="93.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="90" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.5703125" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B2"/>
-      <c r="C2" s="1"/>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="153" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="153" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E81"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="128.5703125" customWidth="1"/>
-    <col min="2" max="2" width="77.28515625" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="75.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="75.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="66.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="66.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="1"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="1"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="1"/>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="1"/>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="1"/>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="1"/>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="1"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="1"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="1"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="1"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="1"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="1"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="1"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="1"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="1"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="1"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="1"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="1"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="1"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="1"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="1"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3782,20 +3794,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794DF495-540A-4416-A570-C2CA3FBB663F}">
-  <dimension ref="A1:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7AB4E8-874D-432E-A74A-D6E3D309D23E}">
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="109.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="86.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="1" max="1" width="105.140625" customWidth="1"/>
+    <col min="2" max="2" width="73.28515625" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3815,40 +3827,40 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>179</v>
+    <row r="2" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>203</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2" t="s">
-        <v>180</v>
+        <v>92</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>193</v>
+    <row r="3" spans="1:5" ht="98.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="215.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -3857,12 +3869,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" t="s">
-        <v>181</v>
+    <row r="5" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3871,40 +3880,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>43</v>
+    <row r="6" spans="1:5" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>182</v>
+    <row r="7" spans="1:5" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>183</v>
+        <v>83</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C8" t="s">
-        <v>184</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="199.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -3913,54 +3925,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="231.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C10" t="s">
-        <v>185</v>
+        <v>84</v>
+      </c>
+      <c r="B9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>79</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>182</v>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
+        <v>131</v>
       </c>
       <c r="C11" t="s">
-        <v>186</v>
+        <v>90</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -3969,12 +3978,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>182</v>
+    <row r="13" spans="1:5" ht="225" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" t="s">
+        <v>131</v>
       </c>
       <c r="C13" t="s">
-        <v>187</v>
+        <v>91</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -3983,92 +3995,80 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>87</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C15" t="s">
-        <v>188</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C16" t="s">
-        <v>189</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="129" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C17" t="s">
-        <v>192</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="265.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C18" t="s">
-        <v>191</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C19" t="s">
-        <v>190</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:5" ht="44.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>